<commit_message>
j'essaie de pousser un conflit
</commit_message>
<xml_diff>
--- a/xls/rpg_2021_chillou.xlsx
+++ b/xls/rpg_2021_chillou.xlsx
@@ -1,16 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/o.prudhomme/Documents/GitHub/Sol_Git/sol_git_1/Aurelien/xls/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0289FF90-D5E4-8D41-AF1D-EA75CB17EFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="620" yWindow="500" windowWidth="28180" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet name="dossier_pac_test__rpg_2021_hb" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="dossier_pac_test__rpg_2021_hb" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="55">
   <si>
     <t>fid</t>
   </si>
@@ -180,29 +190,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="DD/MM/YY" numFmtId="165"/>
-    <numFmt formatCode="DD/MM/YYYY\ HH:MM:SS" numFmtId="166"/>
-    <numFmt formatCode="HH:MM:SS" numFmtId="167"/>
-    <numFmt formatCode="DD/MM/YYYY\ HH:MM:SS.000" numFmtId="168"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="169"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
   </fonts>
-  <fills count="1">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -211,52 +216,336 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="164">
-</xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="164" xfId="0"/>
-    <xf numFmtId="165" xfId="0"/>
-    <xf numFmtId="166" xfId="0"/>
-    <xf numFmtId="167" xfId="0"/>
-    <xf numFmtId="168" xfId="0"/>
-    <xf numFmtId="169" xfId="0"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1024" width="15"/>
-    <col min="2" max="1024" width="15"/>
-    <col min="3" max="1024" width="15"/>
-    <col min="4" max="1024" width="15"/>
-    <col min="5" max="1024" width="15"/>
-    <col min="6" max="1024" width="15"/>
-    <col min="7" max="1024" width="15"/>
-    <col min="8" max="1024" width="15"/>
-    <col min="9" max="1024" width="15"/>
-    <col min="10" max="1024" width="15"/>
-    <col min="11" max="1024" width="15"/>
-    <col min="12" max="1024" width="15"/>
-    <col min="13" max="1024" width="15"/>
-    <col min="14" max="1024" width="15"/>
-    <col min="15" max="1024" width="15"/>
-    <col min="16" max="1024" width="15"/>
-    <col min="17" max="1024" width="15"/>
-    <col min="18" max="1024" width="15"/>
-    <col min="19" max="1024" width="15"/>
-    <col min="20" max="1024" width="15"/>
-    <col min="21" max="1024" width="15"/>
-    <col min="22" max="1024" width="15"/>
-    <col min="23" max="1024" width="15"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -327,7 +616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>2907133</v>
       </c>
@@ -392,7 +681,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2907636</v>
       </c>
@@ -403,7 +692,7 @@
         <v>6.51</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -457,7 +746,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2907646</v>
       </c>
@@ -465,7 +754,7 @@
         <v>38</v>
       </c>
       <c r="C4">
-        <v>4.69</v>
+        <v>4.6900000000000004</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
@@ -522,7 +811,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2907650</v>
       </c>
@@ -587,7 +876,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2907671</v>
       </c>
@@ -652,7 +941,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>2907718</v>
       </c>
@@ -717,7 +1006,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2908388</v>
       </c>
@@ -782,7 +1071,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2908391</v>
       </c>
@@ -847,7 +1136,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2908401</v>
       </c>
@@ -855,7 +1144,7 @@
         <v>53</v>
       </c>
       <c r="C10">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
@@ -912,7 +1201,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:23" ht="13" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2908402</v>
       </c>
@@ -978,5 +1267,6 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>